<commit_message>
SNUxIM increment period by 1 year
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4DD38D8A-2EFB-844F-9D1B-208FD34B1B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B32A08C4-6444-FB42-976E-B4665CE0EEB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1127,9 +1127,6 @@
     <t>DE_GROUP-XUA8pDYjPsw</t>
   </si>
   <si>
-    <t>2019Oct</t>
-  </si>
-  <si>
     <t>GEND_GBV.N.ViolenceServiceType.T.Sexual</t>
   </si>
   <si>
@@ -1272,6 +1269,9 @@
   </si>
   <si>
     <t>QG5SE83IVmL</t>
+  </si>
+  <si>
+    <t>2020Oct</t>
   </si>
 </sst>
 </file>
@@ -2171,10 +2171,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="I91" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2198,7 +2198,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>293</v>
@@ -2266,7 +2266,7 @@
         <v>291</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>361</v>
@@ -2310,7 +2310,7 @@
         <v>291</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>9</v>
@@ -2336,10 +2336,10 @@
         <v>361</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>52</v>
@@ -2354,7 +2354,7 @@
         <v>277</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>89</v>
@@ -2380,10 +2380,10 @@
         <v>361</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>52</v>
@@ -2398,7 +2398,7 @@
         <v>277</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>89</v>
@@ -2418,16 +2418,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>52</v>
@@ -2442,7 +2442,7 @@
         <v>277</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>98</v>
@@ -2468,10 +2468,10 @@
         <v>361</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>52</v>
@@ -2486,7 +2486,7 @@
         <v>276</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>89</v>
@@ -2512,10 +2512,10 @@
         <v>361</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>52</v>
@@ -2530,7 +2530,7 @@
         <v>276</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>89</v>
@@ -2550,16 +2550,16 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>52</v>
@@ -2574,7 +2574,7 @@
         <v>276</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>98</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>361</v>
@@ -2618,7 +2618,7 @@
         <v>272</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>87</v>
@@ -2662,7 +2662,7 @@
         <v>275</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>89</v>
@@ -2706,7 +2706,7 @@
         <v>275</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>89</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>361</v>
@@ -2750,7 +2750,7 @@
         <v>275</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>98</v>
@@ -2794,7 +2794,7 @@
         <v>278</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>89</v>
@@ -2838,7 +2838,7 @@
         <v>278</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>89</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>361</v>
@@ -2882,7 +2882,7 @@
         <v>278</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>98</v>
@@ -2926,7 +2926,7 @@
         <v>282</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>90</v>
@@ -2970,7 +2970,7 @@
         <v>282</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>90</v>
@@ -3014,7 +3014,7 @@
         <v>292</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>89</v>
@@ -3058,7 +3058,7 @@
         <v>292</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>89</v>
@@ -3078,7 +3078,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>361</v>
@@ -3102,7 +3102,7 @@
         <v>292</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>98</v>
@@ -3146,7 +3146,7 @@
         <v>284</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>89</v>
@@ -3190,7 +3190,7 @@
         <v>284</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>89</v>
@@ -3210,7 +3210,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>361</v>
@@ -3234,7 +3234,7 @@
         <v>284</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>98</v>
@@ -3278,7 +3278,7 @@
         <v>285</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>89</v>
@@ -3322,7 +3322,7 @@
         <v>285</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>89</v>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>361</v>
@@ -3366,7 +3366,7 @@
         <v>285</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>98</v>
@@ -3410,7 +3410,7 @@
         <v>286</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>90</v>
@@ -3454,7 +3454,7 @@
         <v>286</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>90</v>
@@ -3492,13 +3492,13 @@
         <v>247</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>89</v>
@@ -3536,13 +3536,13 @@
         <v>247</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>89</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>361</v>
@@ -3580,13 +3580,13 @@
         <v>247</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>98</v>
@@ -3630,7 +3630,7 @@
         <v>288</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>89</v>
@@ -3674,7 +3674,7 @@
         <v>288</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>89</v>
@@ -3694,7 +3694,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>361</v>
@@ -3718,7 +3718,7 @@
         <v>288</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>98</v>
@@ -3762,7 +3762,7 @@
         <v>289</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>89</v>
@@ -3806,7 +3806,7 @@
         <v>289</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>89</v>
@@ -3826,7 +3826,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>361</v>
@@ -3850,7 +3850,7 @@
         <v>289</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>98</v>
@@ -3894,7 +3894,7 @@
         <v>290</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>89</v>
@@ -3938,7 +3938,7 @@
         <v>290</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>89</v>
@@ -3982,7 +3982,7 @@
         <v>281</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>9</v>
@@ -4026,7 +4026,7 @@
         <v>281</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>9</v>
@@ -4046,7 +4046,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>361</v>
@@ -4070,7 +4070,7 @@
         <v>281</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>9</v>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>361</v>
@@ -4114,7 +4114,7 @@
         <v>281</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>9</v>
@@ -4158,7 +4158,7 @@
         <v>287</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>9</v>
@@ -4202,7 +4202,7 @@
         <v>279</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>9</v>
@@ -4246,7 +4246,7 @@
         <v>283</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>9</v>
@@ -4284,13 +4284,13 @@
         <v>247</v>
       </c>
       <c r="G48" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="H48" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>410</v>
-      </c>
       <c r="I48" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>225</v>
@@ -4302,7 +4302,7 @@
         <v>9</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>92</v>
@@ -4328,13 +4328,13 @@
         <v>247</v>
       </c>
       <c r="G49" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="H49" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="H49" s="7" t="s">
-        <v>410</v>
-      </c>
       <c r="I49" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>225</v>
@@ -4346,7 +4346,7 @@
         <v>9</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>92</v>
@@ -4372,13 +4372,13 @@
         <v>247</v>
       </c>
       <c r="G50" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="H50" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="H50" s="4" t="s">
-        <v>370</v>
-      </c>
       <c r="I50" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>87</v>
@@ -4416,13 +4416,13 @@
         <v>247</v>
       </c>
       <c r="G51" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="H51" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="H51" s="4" t="s">
-        <v>370</v>
-      </c>
       <c r="I51" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>87</v>
@@ -4466,7 +4466,7 @@
         <v>269</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>95</v>
@@ -4510,7 +4510,7 @@
         <v>269</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>96</v>
@@ -4554,7 +4554,7 @@
         <v>271</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>87</v>
@@ -4598,7 +4598,7 @@
         <v>274</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>87</v>
@@ -4642,7 +4642,7 @@
         <v>274</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>87</v>
@@ -4686,7 +4686,7 @@
         <v>274</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>87</v>
@@ -4706,7 +4706,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>361</v>
@@ -4730,7 +4730,7 @@
         <v>274</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>98</v>
@@ -4774,7 +4774,7 @@
         <v>271</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>87</v>
@@ -4803,7 +4803,7 @@
         <v>35</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>52</v>
@@ -4818,7 +4818,7 @@
         <v>271</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>98</v>
@@ -4847,7 +4847,7 @@
         <v>35</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>52</v>
@@ -4862,7 +4862,7 @@
         <v>279</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>9</v>
@@ -4906,7 +4906,7 @@
         <v>271</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>98</v>
@@ -4950,7 +4950,7 @@
         <v>279</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>9</v>
@@ -4994,7 +4994,7 @@
         <v>270</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>231</v>
@@ -5038,7 +5038,7 @@
         <v>270</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>231</v>
@@ -5058,7 +5058,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>361</v>
@@ -5079,10 +5079,10 @@
         <v>39</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>295</v>
@@ -5102,7 +5102,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>361</v>
@@ -5123,10 +5123,10 @@
         <v>39</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>295</v>
@@ -5146,7 +5146,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>361</v>
@@ -5167,10 +5167,10 @@
         <v>39</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>295</v>
@@ -5190,7 +5190,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>361</v>
@@ -5211,10 +5211,10 @@
         <v>39</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>295</v>
@@ -5258,7 +5258,7 @@
         <v>271</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>231</v>
@@ -5302,7 +5302,7 @@
         <v>274</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>231</v>
@@ -5346,7 +5346,7 @@
         <v>274</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>231</v>
@@ -5390,7 +5390,7 @@
         <v>274</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>231</v>
@@ -5410,7 +5410,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>361</v>
@@ -5434,7 +5434,7 @@
         <v>274</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>98</v>
@@ -5478,7 +5478,7 @@
         <v>273</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>231</v>
@@ -5522,7 +5522,7 @@
         <v>273</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>231</v>
@@ -5566,7 +5566,7 @@
         <v>280</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>9</v>
@@ -5586,7 +5586,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>361</v>
@@ -5610,7 +5610,7 @@
         <v>280</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>9</v>
@@ -5630,7 +5630,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>361</v>
@@ -5654,7 +5654,7 @@
         <v>280</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>9</v>
@@ -5674,7 +5674,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>361</v>
@@ -5698,7 +5698,7 @@
         <v>280</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>9</v>
@@ -5739,10 +5739,10 @@
         <v>45</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J81" s="4" t="s">
         <v>231</v>
@@ -5783,10 +5783,10 @@
         <v>45</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>231</v>
@@ -5827,10 +5827,10 @@
         <v>47</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J83" s="4" t="s">
         <v>295</v>
@@ -5842,7 +5842,7 @@
         <v>9</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N83" s="4" t="s">
         <v>92</v>
@@ -5871,10 +5871,10 @@
         <v>47</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>295</v>
@@ -5886,7 +5886,7 @@
         <v>9</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>92</v>
@@ -5915,10 +5915,10 @@
         <v>47</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J85" s="4" t="s">
         <v>295</v>
@@ -5930,7 +5930,7 @@
         <v>9</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>92</v>
@@ -5959,10 +5959,10 @@
         <v>47</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J86" s="4" t="s">
         <v>295</v>
@@ -5974,7 +5974,7 @@
         <v>9</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>92</v>
@@ -6006,7 +6006,7 @@
         <v>273</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>98</v>
@@ -6018,7 +6018,7 @@
         <v>9</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>92</v>
@@ -6050,7 +6050,7 @@
         <v>273</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>98</v>
@@ -6062,7 +6062,7 @@
         <v>9</v>
       </c>
       <c r="M88" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N88" s="4" t="s">
         <v>92</v>
@@ -6070,7 +6070,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>361</v>
@@ -6094,7 +6094,7 @@
         <v>273</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>98</v>
@@ -6106,7 +6106,7 @@
         <v>9</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N89" s="4" t="s">
         <v>92</v>
@@ -6138,7 +6138,7 @@
         <v>273</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J90" s="4" t="s">
         <v>98</v>
@@ -6150,7 +6150,7 @@
         <v>9</v>
       </c>
       <c r="M90" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>92</v>
@@ -6158,7 +6158,7 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>361</v>
@@ -6167,7 +6167,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>52</v>
@@ -6182,7 +6182,7 @@
         <v>273</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
change snuXim configuration to use de group for 21T
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B32A08C4-6444-FB42-976E-B4665CE0EEB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ECB67BB4-7C17-B44D-953C-CBEDAA2FE64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1124,9 +1124,6 @@
     <t>VMMC_CIRC.N.Age_Sex_HIVStatus.T.Unknown</t>
   </si>
   <si>
-    <t>DE_GROUP-XUA8pDYjPsw</t>
-  </si>
-  <si>
     <t>GEND_GBV.N.ViolenceServiceType.T.Sexual</t>
   </si>
   <si>
@@ -1272,6 +1269,9 @@
   </si>
   <si>
     <t>2020Oct</t>
+  </si>
+  <si>
+    <t>DE_GROUP-WTq0quAW1mf</t>
   </si>
 </sst>
 </file>
@@ -2171,10 +2171,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="I91" sqref="I1:I1048576"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2:B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2198,7 +2198,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>293</v>
@@ -2245,7 +2245,7 @@
         <v>296</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
@@ -2266,7 +2266,7 @@
         <v>291</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>
@@ -2286,10 +2286,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -2310,7 +2310,7 @@
         <v>291</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>9</v>
@@ -2333,13 +2333,13 @@
         <v>304</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>52</v>
@@ -2354,7 +2354,7 @@
         <v>277</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>89</v>
@@ -2377,13 +2377,13 @@
         <v>305</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>52</v>
@@ -2398,7 +2398,7 @@
         <v>277</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>89</v>
@@ -2418,16 +2418,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>52</v>
@@ -2442,7 +2442,7 @@
         <v>277</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>98</v>
@@ -2465,13 +2465,13 @@
         <v>306</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>52</v>
@@ -2486,7 +2486,7 @@
         <v>276</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>89</v>
@@ -2509,13 +2509,13 @@
         <v>307</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>52</v>
@@ -2530,7 +2530,7 @@
         <v>276</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>89</v>
@@ -2550,16 +2550,16 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>52</v>
@@ -2574,7 +2574,7 @@
         <v>276</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>98</v>
@@ -2594,10 +2594,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
@@ -2618,7 +2618,7 @@
         <v>272</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>87</v>
@@ -2641,7 +2641,7 @@
         <v>308</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>20</v>
@@ -2662,7 +2662,7 @@
         <v>275</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>89</v>
@@ -2685,7 +2685,7 @@
         <v>309</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>20</v>
@@ -2706,7 +2706,7 @@
         <v>275</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>89</v>
@@ -2726,10 +2726,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>20</v>
@@ -2750,7 +2750,7 @@
         <v>275</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>98</v>
@@ -2773,7 +2773,7 @@
         <v>310</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>20</v>
@@ -2794,7 +2794,7 @@
         <v>278</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>89</v>
@@ -2817,7 +2817,7 @@
         <v>311</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>20</v>
@@ -2838,7 +2838,7 @@
         <v>278</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>89</v>
@@ -2858,10 +2858,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>20</v>
@@ -2882,7 +2882,7 @@
         <v>278</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>98</v>
@@ -2905,7 +2905,7 @@
         <v>312</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>20</v>
@@ -2926,7 +2926,7 @@
         <v>282</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>90</v>
@@ -2949,7 +2949,7 @@
         <v>313</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>20</v>
@@ -2970,7 +2970,7 @@
         <v>282</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>90</v>
@@ -2993,7 +2993,7 @@
         <v>314</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>20</v>
@@ -3014,7 +3014,7 @@
         <v>292</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>89</v>
@@ -3037,7 +3037,7 @@
         <v>315</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>20</v>
@@ -3058,7 +3058,7 @@
         <v>292</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>89</v>
@@ -3078,10 +3078,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>20</v>
@@ -3102,7 +3102,7 @@
         <v>292</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>98</v>
@@ -3125,7 +3125,7 @@
         <v>316</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>20</v>
@@ -3146,7 +3146,7 @@
         <v>284</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>89</v>
@@ -3169,7 +3169,7 @@
         <v>317</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>20</v>
@@ -3190,7 +3190,7 @@
         <v>284</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>89</v>
@@ -3210,10 +3210,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>20</v>
@@ -3234,7 +3234,7 @@
         <v>284</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>98</v>
@@ -3257,7 +3257,7 @@
         <v>318</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>20</v>
@@ -3278,7 +3278,7 @@
         <v>285</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>89</v>
@@ -3301,7 +3301,7 @@
         <v>319</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>20</v>
@@ -3322,7 +3322,7 @@
         <v>285</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>89</v>
@@ -3342,10 +3342,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>20</v>
@@ -3366,7 +3366,7 @@
         <v>285</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>98</v>
@@ -3389,7 +3389,7 @@
         <v>320</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>20</v>
@@ -3410,7 +3410,7 @@
         <v>286</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>90</v>
@@ -3433,7 +3433,7 @@
         <v>321</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>20</v>
@@ -3454,7 +3454,7 @@
         <v>286</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>90</v>
@@ -3477,7 +3477,7 @@
         <v>322</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>20</v>
@@ -3492,13 +3492,13 @@
         <v>247</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>89</v>
@@ -3521,7 +3521,7 @@
         <v>323</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>20</v>
@@ -3536,13 +3536,13 @@
         <v>247</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>89</v>
@@ -3562,10 +3562,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>20</v>
@@ -3580,13 +3580,13 @@
         <v>247</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>98</v>
@@ -3609,7 +3609,7 @@
         <v>324</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>20</v>
@@ -3630,7 +3630,7 @@
         <v>288</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>89</v>
@@ -3653,7 +3653,7 @@
         <v>325</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>20</v>
@@ -3674,7 +3674,7 @@
         <v>288</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>89</v>
@@ -3694,10 +3694,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>20</v>
@@ -3718,7 +3718,7 @@
         <v>288</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>98</v>
@@ -3741,7 +3741,7 @@
         <v>326</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
@@ -3762,7 +3762,7 @@
         <v>289</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>89</v>
@@ -3785,7 +3785,7 @@
         <v>327</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>20</v>
@@ -3806,7 +3806,7 @@
         <v>289</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>89</v>
@@ -3826,10 +3826,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>20</v>
@@ -3850,7 +3850,7 @@
         <v>289</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>98</v>
@@ -3873,7 +3873,7 @@
         <v>328</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>20</v>
@@ -3894,7 +3894,7 @@
         <v>290</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>89</v>
@@ -3917,7 +3917,7 @@
         <v>329</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>20</v>
@@ -3938,7 +3938,7 @@
         <v>290</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>89</v>
@@ -3961,7 +3961,7 @@
         <v>330</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>20</v>
@@ -3982,7 +3982,7 @@
         <v>281</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>9</v>
@@ -4005,7 +4005,7 @@
         <v>331</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>20</v>
@@ -4026,7 +4026,7 @@
         <v>281</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>9</v>
@@ -4046,10 +4046,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>20</v>
@@ -4070,7 +4070,7 @@
         <v>281</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>9</v>
@@ -4090,10 +4090,10 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>20</v>
@@ -4114,7 +4114,7 @@
         <v>281</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>9</v>
@@ -4137,7 +4137,7 @@
         <v>297</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>22</v>
@@ -4158,7 +4158,7 @@
         <v>287</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>9</v>
@@ -4181,7 +4181,7 @@
         <v>298</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>24</v>
@@ -4202,7 +4202,7 @@
         <v>279</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>9</v>
@@ -4225,7 +4225,7 @@
         <v>299</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>26</v>
@@ -4246,7 +4246,7 @@
         <v>283</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>9</v>
@@ -4269,7 +4269,7 @@
         <v>332</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>27</v>
@@ -4284,13 +4284,13 @@
         <v>247</v>
       </c>
       <c r="G48" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="H48" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>409</v>
-      </c>
       <c r="I48" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>225</v>
@@ -4302,7 +4302,7 @@
         <v>9</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>92</v>
@@ -4313,7 +4313,7 @@
         <v>333</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>27</v>
@@ -4328,13 +4328,13 @@
         <v>247</v>
       </c>
       <c r="G49" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="H49" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="H49" s="7" t="s">
-        <v>409</v>
-      </c>
       <c r="I49" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>225</v>
@@ -4346,7 +4346,7 @@
         <v>9</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>92</v>
@@ -4357,7 +4357,7 @@
         <v>334</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>28</v>
@@ -4372,13 +4372,13 @@
         <v>247</v>
       </c>
       <c r="G50" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="H50" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="H50" s="4" t="s">
-        <v>369</v>
-      </c>
       <c r="I50" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>87</v>
@@ -4401,7 +4401,7 @@
         <v>335</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>28</v>
@@ -4416,13 +4416,13 @@
         <v>247</v>
       </c>
       <c r="G51" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="H51" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="H51" s="4" t="s">
-        <v>369</v>
-      </c>
       <c r="I51" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>87</v>
@@ -4445,7 +4445,7 @@
         <v>300</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>29</v>
@@ -4466,7 +4466,7 @@
         <v>269</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>95</v>
@@ -4489,7 +4489,7 @@
         <v>301</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>29</v>
@@ -4510,7 +4510,7 @@
         <v>269</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>96</v>
@@ -4533,7 +4533,7 @@
         <v>336</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>31</v>
@@ -4554,7 +4554,7 @@
         <v>271</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>87</v>
@@ -4577,7 +4577,7 @@
         <v>337</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>31</v>
@@ -4598,7 +4598,7 @@
         <v>274</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>87</v>
@@ -4621,7 +4621,7 @@
         <v>338</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>31</v>
@@ -4642,7 +4642,7 @@
         <v>274</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>87</v>
@@ -4665,7 +4665,7 @@
         <v>339</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>31</v>
@@ -4686,7 +4686,7 @@
         <v>274</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>87</v>
@@ -4706,10 +4706,10 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>31</v>
@@ -4730,7 +4730,7 @@
         <v>274</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>98</v>
@@ -4753,7 +4753,7 @@
         <v>340</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>34</v>
@@ -4774,7 +4774,7 @@
         <v>271</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>87</v>
@@ -4797,13 +4797,13 @@
         <v>341</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>52</v>
@@ -4818,7 +4818,7 @@
         <v>271</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>98</v>
@@ -4841,13 +4841,13 @@
         <v>302</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>52</v>
@@ -4862,7 +4862,7 @@
         <v>279</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>9</v>
@@ -4885,7 +4885,7 @@
         <v>342</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>36</v>
@@ -4906,7 +4906,7 @@
         <v>271</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>98</v>
@@ -4929,7 +4929,7 @@
         <v>303</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>36</v>
@@ -4950,7 +4950,7 @@
         <v>279</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>9</v>
@@ -4973,7 +4973,7 @@
         <v>343</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>37</v>
@@ -4994,7 +4994,7 @@
         <v>270</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>231</v>
@@ -5017,7 +5017,7 @@
         <v>344</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>37</v>
@@ -5038,7 +5038,7 @@
         <v>270</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>231</v>
@@ -5058,10 +5058,10 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>38</v>
@@ -5079,10 +5079,10 @@
         <v>39</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>295</v>
@@ -5102,10 +5102,10 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>38</v>
@@ -5123,10 +5123,10 @@
         <v>39</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>295</v>
@@ -5146,10 +5146,10 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>38</v>
@@ -5167,10 +5167,10 @@
         <v>39</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>295</v>
@@ -5190,10 +5190,10 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>38</v>
@@ -5211,10 +5211,10 @@
         <v>39</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>295</v>
@@ -5237,7 +5237,7 @@
         <v>345</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>40</v>
@@ -5258,7 +5258,7 @@
         <v>271</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>231</v>
@@ -5281,7 +5281,7 @@
         <v>346</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>40</v>
@@ -5302,7 +5302,7 @@
         <v>274</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>231</v>
@@ -5325,7 +5325,7 @@
         <v>347</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>40</v>
@@ -5346,7 +5346,7 @@
         <v>274</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>231</v>
@@ -5369,7 +5369,7 @@
         <v>348</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>40</v>
@@ -5390,7 +5390,7 @@
         <v>274</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>231</v>
@@ -5410,10 +5410,10 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>40</v>
@@ -5434,7 +5434,7 @@
         <v>274</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>98</v>
@@ -5457,7 +5457,7 @@
         <v>349</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>41</v>
@@ -5478,7 +5478,7 @@
         <v>273</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>231</v>
@@ -5501,7 +5501,7 @@
         <v>350</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>42</v>
@@ -5522,7 +5522,7 @@
         <v>273</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>231</v>
@@ -5545,7 +5545,7 @@
         <v>351</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>42</v>
@@ -5566,7 +5566,7 @@
         <v>280</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>9</v>
@@ -5586,10 +5586,10 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>42</v>
@@ -5610,7 +5610,7 @@
         <v>280</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>9</v>
@@ -5630,10 +5630,10 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>42</v>
@@ -5654,7 +5654,7 @@
         <v>280</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>9</v>
@@ -5674,10 +5674,10 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>42</v>
@@ -5698,7 +5698,7 @@
         <v>280</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>9</v>
@@ -5721,7 +5721,7 @@
         <v>352</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>44</v>
@@ -5739,10 +5739,10 @@
         <v>45</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J81" s="4" t="s">
         <v>231</v>
@@ -5765,7 +5765,7 @@
         <v>353</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>44</v>
@@ -5783,10 +5783,10 @@
         <v>45</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>231</v>
@@ -5809,7 +5809,7 @@
         <v>354</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>46</v>
@@ -5827,10 +5827,10 @@
         <v>47</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J83" s="4" t="s">
         <v>295</v>
@@ -5842,7 +5842,7 @@
         <v>9</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N83" s="4" t="s">
         <v>92</v>
@@ -5853,7 +5853,7 @@
         <v>355</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>46</v>
@@ -5871,10 +5871,10 @@
         <v>47</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>295</v>
@@ -5886,7 +5886,7 @@
         <v>9</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>92</v>
@@ -5897,7 +5897,7 @@
         <v>356</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>46</v>
@@ -5915,10 +5915,10 @@
         <v>47</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J85" s="4" t="s">
         <v>295</v>
@@ -5930,7 +5930,7 @@
         <v>9</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>92</v>
@@ -5941,7 +5941,7 @@
         <v>357</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>46</v>
@@ -5959,10 +5959,10 @@
         <v>47</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J86" s="4" t="s">
         <v>295</v>
@@ -5974,7 +5974,7 @@
         <v>9</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>92</v>
@@ -5985,7 +5985,7 @@
         <v>358</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>48</v>
@@ -6006,7 +6006,7 @@
         <v>273</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>98</v>
@@ -6018,7 +6018,7 @@
         <v>9</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>92</v>
@@ -6029,7 +6029,7 @@
         <v>359</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>48</v>
@@ -6050,7 +6050,7 @@
         <v>273</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>98</v>
@@ -6062,7 +6062,7 @@
         <v>9</v>
       </c>
       <c r="M88" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N88" s="4" t="s">
         <v>92</v>
@@ -6070,10 +6070,10 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>48</v>
@@ -6094,7 +6094,7 @@
         <v>273</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>98</v>
@@ -6106,7 +6106,7 @@
         <v>9</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N89" s="4" t="s">
         <v>92</v>
@@ -6117,7 +6117,7 @@
         <v>360</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>48</v>
@@ -6138,7 +6138,7 @@
         <v>273</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J90" s="4" t="s">
         <v>98</v>
@@ -6150,7 +6150,7 @@
         <v>9</v>
       </c>
       <c r="M90" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>92</v>
@@ -6158,16 +6158,16 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>52</v>
@@ -6182,7 +6182,7 @@
         <v>273</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Updated indicator codes in column A
Updated indicator codes in column A
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christiandomaas/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ECB67BB4-7C17-B44D-953C-CBEDAA2FE64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C14A492F-1CEE-2C41-B463-C3A89658D49C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35080" yWindow="980" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1638" uniqueCount="411">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1638" uniqueCount="409">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -929,207 +929,6 @@
     <t>&lt;15/&gt;15</t>
   </si>
   <si>
-    <t>GEND_GBV.N.ViolenceServiceType.T.physEmot</t>
-  </si>
-  <si>
-    <t>KP_MAT.N.Sex.T</t>
-  </si>
-  <si>
-    <t>KP_PREV.N.KeyPop.T</t>
-  </si>
-  <si>
-    <t>OVC_HIVSTAT.N.total.T</t>
-  </si>
-  <si>
-    <t>PMTCT_EID.N.Age.T.2mo</t>
-  </si>
-  <si>
-    <t>PMTCT_EID.N.Age.T.2to12mo</t>
-  </si>
-  <si>
-    <t>PrEP_CURR.N.KeyPop.T</t>
-  </si>
-  <si>
-    <t>PrEP_NEW.N.KeyPop.T</t>
-  </si>
-  <si>
-    <t>HTS_INDEX_COM.N.Age_Sex_Result.T.NewNeg</t>
-  </si>
-  <si>
-    <t>HTS_INDEX_COM.N.Age_Sex_Result.T.NewPos</t>
-  </si>
-  <si>
-    <t>HTS_INDEX_FAC.N.Age_Sex_Result.T.NewNeg</t>
-  </si>
-  <si>
-    <t>HTS_INDEX_FAC.N.Age_Sex_Result.T.NewPos</t>
-  </si>
-  <si>
-    <t>HTS_TST_EmergencyWard.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_EmergencyWard.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_Inpat.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_Inpat.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_Malnutrition.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_Malnutrition.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_MobileMod.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_MobileMod.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_OtherMod.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_OtherMod.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_OtherPITC.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_OtherPITC.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_Pediatric.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_Pediatric.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_PMTCTPostANC1.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_PMTCTPostANC1.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_STIClinic.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_STIClinic.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_VCT.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_VCT.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST_VCTMod.N.Age_Sex_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST_VCTMod.N.Age_Sex_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>HTS_TST.N.KeyPop_Result.T.Negative</t>
-  </si>
-  <si>
-    <t>HTS_TST.N.KeyPop_Result.T.Positive</t>
-  </si>
-  <si>
-    <t>OVC_SERV.N.Age_Sex_ProgramStatus.T.Active</t>
-  </si>
-  <si>
-    <t>OVC_SERV.N.Age_Sex_ProgramStatus.T.Graduated</t>
-  </si>
-  <si>
-    <t>PMTCT_ART.N.Age_NewExistingART_Sex_HIVStatus.T.Already</t>
-  </si>
-  <si>
-    <t>PMTCT_ART.N.Age_NewExistingART_Sex_HIVStatus.T.New</t>
-  </si>
-  <si>
-    <t>PMTCT_STAT.D.Age_Sex.T</t>
-  </si>
-  <si>
-    <t>PMTCT_STAT.N.Age_Sex_KnownNewResult.T.KnownPos</t>
-  </si>
-  <si>
-    <t>PMTCT_STAT.N.Age_Sex_KnownNewResult.T.NewNeg</t>
-  </si>
-  <si>
-    <t>PMTCT_STAT.N.Age_Sex_KnownNewResult.T.NewPos</t>
-  </si>
-  <si>
-    <t>PP_PREV.N.Age_Sex.T</t>
-  </si>
-  <si>
-    <t>PrEP_CURR.N.Age_Sex.T</t>
-  </si>
-  <si>
-    <t>PrEP_NEW.N.Age_Sex.T</t>
-  </si>
-  <si>
-    <t>TB_ART.N.Age_Sex_NewExistingART_HIVStatus.T.Already</t>
-  </si>
-  <si>
-    <t>TB_ART.N.Age_Sex_NewExistingART_HIVStatus.T.New</t>
-  </si>
-  <si>
-    <t>TB_STAT.D.Age_Sex.T</t>
-  </si>
-  <si>
-    <t>TB_STAT.N.Age_Sex_KnownNewPosNeg.T.KnownPos</t>
-  </si>
-  <si>
-    <t>TB_STAT.N.Age_Sex_KnownNewPosNeg.T.NewNeg</t>
-  </si>
-  <si>
-    <t>TB_STAT.N.Age_Sex_KnownNewPosNeg.T.NewPos</t>
-  </si>
-  <si>
-    <t>TX_CURR.N.Age_Sex_HIVStatus.T</t>
-  </si>
-  <si>
-    <t>TX_NEW.N.Age_Sex_HIVStatus.T</t>
-  </si>
-  <si>
-    <t>TX_NEW.N.KeyPop_HIVStatus.T</t>
-  </si>
-  <si>
-    <t>TX_PVLS.D.Age_Sex_Indication_HIVStatus.T.Routine</t>
-  </si>
-  <si>
-    <t>TX_PVLS.N.Age_Sex_Indication_HIVStatus.T.Routine</t>
-  </si>
-  <si>
-    <t>TX_TB.D.Age_Sex_TBScreen_NewExistingART_HIVStatus.T.ScreenNegAlready</t>
-  </si>
-  <si>
-    <t>TX_TB.D.Age_Sex_TBScreen_NewExistingART_HIVStatus.T.ScreenNegNew</t>
-  </si>
-  <si>
-    <t>TX_TB.D.Age_Sex_TBScreen_NewExistingART_HIVStatus.T.ScreenPosAlready</t>
-  </si>
-  <si>
-    <t>TX_TB.D.Age_Sex_TBScreen_NewExistingART_HIVStatus.T.ScreenPosNew</t>
-  </si>
-  <si>
-    <t>VMMC_CIRC.N.Age_Sex_HIVStatus.T.Negative</t>
-  </si>
-  <si>
-    <t>VMMC_CIRC.N.Age_Sex_HIVStatus.T.Positive</t>
-  </si>
-  <si>
-    <t>VMMC_CIRC.N.Age_Sex_HIVStatus.T.Unknown</t>
-  </si>
-  <si>
-    <t>GEND_GBV.N.ViolenceServiceType.T.Sexual</t>
-  </si>
-  <si>
-    <t>HTS_SELF.N.Age_Sex_HIVSelfTest.T</t>
-  </si>
-  <si>
     <t>HTS_INDEX</t>
   </si>
   <si>
@@ -1151,18 +950,6 @@
     <t>ClkvX1lYY12</t>
   </si>
   <si>
-    <t>TB_PREV.D.Age_NewExistingArt_HIVStatus.T.New</t>
-  </si>
-  <si>
-    <t>TB_PREV.D.Age_NewExistingArt_HIVStatus.T.Already</t>
-  </si>
-  <si>
-    <t>TB_PREV.N.Age_NewExistingArt_HIVStatus.T.New</t>
-  </si>
-  <si>
-    <t>TB_PREV.N.Age_NewExistingArt_HIVStatus.T.Already</t>
-  </si>
-  <si>
     <t>pkZRNlMgL89</t>
   </si>
   <si>
@@ -1193,75 +980,18 @@
     <t>tb_p_art_n</t>
   </si>
   <si>
-    <t>CXCA_SCRN.N.Age_Sex_HIVStatus.T</t>
-  </si>
-  <si>
     <t>qOgXk080fJH</t>
   </si>
   <si>
     <t>indicator_code</t>
   </si>
   <si>
-    <t>HTS_RECENT_IndexMod.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_Index.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_Inpat.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_TB.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_PMTCT.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_PMTCTPostANC1.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_VMMC.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_STIClinic.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_Emergency.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_OtherPITC.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_VCT.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_MobileMod.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT_OtherMod.N.Age_Sex_Result.T</t>
-  </si>
-  <si>
-    <t>HTS_RECENT.N.KeyPop_HIVStatus.T</t>
-  </si>
-  <si>
     <t>PTL2kxpEOg3</t>
   </si>
   <si>
     <t>PMTCT PostANC/Age/Sex/Result</t>
   </si>
   <si>
-    <t>HTS_SELF.N.KeyPop.T</t>
-  </si>
-  <si>
-    <t>TX_CURR.N.KeyPop_HIVStatus.T</t>
-  </si>
-  <si>
-    <t>TX_PVLS.D.KeyPop_HIVStatus.T</t>
-  </si>
-  <si>
-    <t>TX_PVLS.N.KeyPop_HIVStatus.T</t>
-  </si>
-  <si>
     <t>Age/Sex/ProgramStatus</t>
   </si>
   <si>
@@ -1272,6 +1002,270 @@
   </si>
   <si>
     <t>DE_GROUP-WTq0quAW1mf</t>
+  </si>
+  <si>
+    <t>GEND_GBV.PE.T</t>
+  </si>
+  <si>
+    <t>GEND_GBV.S.T</t>
+  </si>
+  <si>
+    <t>HTS_INDEX_COM.New.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_INDEX_COM.New.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.IndexCom.T</t>
+  </si>
+  <si>
+    <t>HTS_INDEX_FAC.New.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_INDEX_FAC.New.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.IndexFac.T</t>
+  </si>
+  <si>
+    <t>HTS_SELF.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.EW.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.EW.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.EW.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.Inpat.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.Inpat.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.Inpat.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.Maln.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.Maln.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.MobileCom.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.MobileCom.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.MobileCom.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.OtherCom.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.OtherCom.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.OtherCom.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.Other.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.Other.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.Other.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.Peds.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.Peds.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.PostANC1.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.PostANC1.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.PostANC1.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.STI.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.STI.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.STI.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.VCT.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.VCT.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.VCT.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.KP.Neg.T</t>
+  </si>
+  <si>
+    <t>HTS_TST.KP.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_SELF.KP.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.KP.T</t>
+  </si>
+  <si>
+    <t>KP_MAT.T</t>
+  </si>
+  <si>
+    <t>KP_PREV.T</t>
+  </si>
+  <si>
+    <t>OVC_HIVSTAT.T</t>
+  </si>
+  <si>
+    <t>OVC_SERV.Active.T</t>
+  </si>
+  <si>
+    <t>OVC_SERV.Graduated.T</t>
+  </si>
+  <si>
+    <t>PMTCT_ART.Already.T</t>
+  </si>
+  <si>
+    <t>PMTCT_ART.New.T</t>
+  </si>
+  <si>
+    <t>PMTCT_EID.N.2.T</t>
+  </si>
+  <si>
+    <t>PMTCT_EID.N.12.T</t>
+  </si>
+  <si>
+    <t>PMTCT_STAT.D.T</t>
+  </si>
+  <si>
+    <t>PMTCT_STAT.N.KnownPos.T</t>
+  </si>
+  <si>
+    <t>PMTCT_STAT.N.New.Neg.T</t>
+  </si>
+  <si>
+    <t>PMTCT_STAT.N.New.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.PMTCT.T</t>
+  </si>
+  <si>
+    <t>PP_PREV.T</t>
+  </si>
+  <si>
+    <t>PrEP_CURR.T</t>
+  </si>
+  <si>
+    <t>PrEP_CURR.KP.T</t>
+  </si>
+  <si>
+    <t>PrEP_NEW.T</t>
+  </si>
+  <si>
+    <t>PrEP_NEW.KP.T</t>
+  </si>
+  <si>
+    <t>TB_ART.Already.T</t>
+  </si>
+  <si>
+    <t>TB_ART.New.T</t>
+  </si>
+  <si>
+    <t>TB_PREV.D.Already.T</t>
+  </si>
+  <si>
+    <t>TB_PREV.D.New.T</t>
+  </si>
+  <si>
+    <t>TB_PREV.N.Already.T</t>
+  </si>
+  <si>
+    <t>TB_PREV.N.New.T</t>
+  </si>
+  <si>
+    <t>TB_STAT.D.T</t>
+  </si>
+  <si>
+    <t>TB_STAT.N.KnownPos.T</t>
+  </si>
+  <si>
+    <t>TB_STAT.N.New.Neg.T</t>
+  </si>
+  <si>
+    <t>TB_STAT.N.New.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.TB.T</t>
+  </si>
+  <si>
+    <t>TX_CURR.T</t>
+  </si>
+  <si>
+    <t>TX_NEW.T</t>
+  </si>
+  <si>
+    <t>TX_NEW.KP.T</t>
+  </si>
+  <si>
+    <t>TX_CURR.KP.T</t>
+  </si>
+  <si>
+    <t>TX_PVLS.D.KP.T</t>
+  </si>
+  <si>
+    <t>TX_PVLS.N.KP.T</t>
+  </si>
+  <si>
+    <t>TX_PVLS.D.Routine.T</t>
+  </si>
+  <si>
+    <t>TX_PVLS.N.Routine.T</t>
+  </si>
+  <si>
+    <t>TX_TB.D.Already.Neg.T</t>
+  </si>
+  <si>
+    <t>TX_TB.D.New.Neg.T</t>
+  </si>
+  <si>
+    <t>TX_TB.D.Already.Pos.T</t>
+  </si>
+  <si>
+    <t>TX_TB.D.New.Pos.T</t>
+  </si>
+  <si>
+    <t>VMMC_CIRC.Neg.T</t>
+  </si>
+  <si>
+    <t>VMMC_CIRC.Pos.T</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.VMMC.T</t>
+  </si>
+  <si>
+    <t>VMMC_CIRC.Unk.T</t>
+  </si>
+  <si>
+    <t>CXCA_SCRN.T</t>
   </si>
 </sst>
 </file>
@@ -2171,10 +2165,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:B91"/>
+      <selection pane="topRight" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2198,7 +2192,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>386</v>
+        <v>314</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>293</v>
@@ -2242,10 +2236,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
@@ -2266,7 +2260,7 @@
         <v>291</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>
@@ -2286,10 +2280,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>361</v>
+        <v>322</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -2310,7 +2304,7 @@
         <v>291</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>9</v>
@@ -2330,16 +2324,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>363</v>
+        <v>296</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>364</v>
+        <v>297</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>52</v>
@@ -2354,7 +2348,7 @@
         <v>277</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>89</v>
@@ -2374,16 +2368,16 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>363</v>
+        <v>296</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>364</v>
+        <v>297</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>52</v>
@@ -2398,7 +2392,7 @@
         <v>277</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>89</v>
@@ -2418,16 +2412,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>387</v>
+        <v>325</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>363</v>
+        <v>296</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>364</v>
+        <v>297</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>52</v>
@@ -2442,7 +2436,7 @@
         <v>277</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>98</v>
@@ -2462,16 +2456,16 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>363</v>
+        <v>296</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>364</v>
+        <v>297</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>52</v>
@@ -2486,7 +2480,7 @@
         <v>276</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>89</v>
@@ -2506,16 +2500,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>363</v>
+        <v>296</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>364</v>
+        <v>297</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>52</v>
@@ -2530,7 +2524,7 @@
         <v>276</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>89</v>
@@ -2550,16 +2544,16 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>388</v>
+        <v>328</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>363</v>
+        <v>296</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>364</v>
+        <v>297</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>52</v>
@@ -2574,7 +2568,7 @@
         <v>276</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>98</v>
@@ -2594,10 +2588,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>362</v>
+        <v>329</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
@@ -2618,7 +2612,7 @@
         <v>272</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>87</v>
@@ -2638,10 +2632,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>20</v>
@@ -2662,7 +2656,7 @@
         <v>275</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>89</v>
@@ -2682,10 +2676,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>20</v>
@@ -2706,7 +2700,7 @@
         <v>275</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>89</v>
@@ -2726,10 +2720,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>395</v>
+        <v>332</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>20</v>
@@ -2750,7 +2744,7 @@
         <v>275</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>98</v>
@@ -2770,10 +2764,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>20</v>
@@ -2794,7 +2788,7 @@
         <v>278</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>89</v>
@@ -2814,10 +2808,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>20</v>
@@ -2838,7 +2832,7 @@
         <v>278</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>89</v>
@@ -2858,10 +2852,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>389</v>
+        <v>335</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>20</v>
@@ -2882,7 +2876,7 @@
         <v>278</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>98</v>
@@ -2902,10 +2896,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>312</v>
+        <v>336</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>20</v>
@@ -2926,7 +2920,7 @@
         <v>282</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>90</v>
@@ -2946,10 +2940,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>313</v>
+        <v>337</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>20</v>
@@ -2970,7 +2964,7 @@
         <v>282</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>90</v>
@@ -2990,10 +2984,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>20</v>
@@ -3014,7 +3008,7 @@
         <v>292</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>89</v>
@@ -3034,10 +3028,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>315</v>
+        <v>339</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>20</v>
@@ -3058,7 +3052,7 @@
         <v>292</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>89</v>
@@ -3078,10 +3072,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>398</v>
+        <v>340</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>20</v>
@@ -3102,7 +3096,7 @@
         <v>292</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>98</v>
@@ -3122,10 +3116,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>20</v>
@@ -3146,7 +3140,7 @@
         <v>284</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>89</v>
@@ -3166,10 +3160,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>20</v>
@@ -3190,7 +3184,7 @@
         <v>284</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>89</v>
@@ -3210,10 +3204,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>399</v>
+        <v>343</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>20</v>
@@ -3234,7 +3228,7 @@
         <v>284</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>98</v>
@@ -3254,10 +3248,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>20</v>
@@ -3278,7 +3272,7 @@
         <v>285</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>89</v>
@@ -3298,10 +3292,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>20</v>
@@ -3322,7 +3316,7 @@
         <v>285</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>89</v>
@@ -3342,10 +3336,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>20</v>
@@ -3366,7 +3360,7 @@
         <v>285</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>98</v>
@@ -3386,10 +3380,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>20</v>
@@ -3410,7 +3404,7 @@
         <v>286</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>90</v>
@@ -3430,10 +3424,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>20</v>
@@ -3454,7 +3448,7 @@
         <v>286</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>90</v>
@@ -3474,10 +3468,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>322</v>
+        <v>349</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>20</v>
@@ -3492,13 +3486,13 @@
         <v>247</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>402</v>
+        <v>316</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>401</v>
+        <v>315</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>89</v>
@@ -3518,10 +3512,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>323</v>
+        <v>350</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>20</v>
@@ -3536,13 +3530,13 @@
         <v>247</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>402</v>
+        <v>316</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>401</v>
+        <v>315</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>89</v>
@@ -3562,10 +3556,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>392</v>
+        <v>351</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>20</v>
@@ -3580,13 +3574,13 @@
         <v>247</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>402</v>
+        <v>316</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>401</v>
+        <v>315</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>98</v>
@@ -3606,10 +3600,10 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>324</v>
+        <v>352</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>20</v>
@@ -3630,7 +3624,7 @@
         <v>288</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>89</v>
@@ -3650,10 +3644,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>325</v>
+        <v>353</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>20</v>
@@ -3674,7 +3668,7 @@
         <v>288</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>89</v>
@@ -3694,10 +3688,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>394</v>
+        <v>354</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>20</v>
@@ -3718,7 +3712,7 @@
         <v>288</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>98</v>
@@ -3738,10 +3732,10 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>326</v>
+        <v>355</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
@@ -3762,7 +3756,7 @@
         <v>289</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>89</v>
@@ -3782,10 +3776,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>20</v>
@@ -3806,7 +3800,7 @@
         <v>289</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>89</v>
@@ -3826,10 +3820,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>20</v>
@@ -3850,7 +3844,7 @@
         <v>289</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>98</v>
@@ -3870,10 +3864,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>328</v>
+        <v>355</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>20</v>
@@ -3894,7 +3888,7 @@
         <v>290</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>89</v>
@@ -3914,10 +3908,10 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>329</v>
+        <v>356</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>20</v>
@@ -3938,7 +3932,7 @@
         <v>290</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>89</v>
@@ -3958,10 +3952,10 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>330</v>
+        <v>358</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>20</v>
@@ -3982,7 +3976,7 @@
         <v>281</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>9</v>
@@ -4002,10 +3996,10 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>331</v>
+        <v>359</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>20</v>
@@ -4026,7 +4020,7 @@
         <v>281</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>9</v>
@@ -4046,10 +4040,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>20</v>
@@ -4070,7 +4064,7 @@
         <v>281</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>9</v>
@@ -4090,10 +4084,10 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>20</v>
@@ -4114,7 +4108,7 @@
         <v>281</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>9</v>
@@ -4134,10 +4128,10 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>297</v>
+        <v>362</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>22</v>
@@ -4158,7 +4152,7 @@
         <v>287</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>9</v>
@@ -4178,10 +4172,10 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>298</v>
+        <v>363</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>24</v>
@@ -4202,7 +4196,7 @@
         <v>279</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>9</v>
@@ -4222,10 +4216,10 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>299</v>
+        <v>364</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>26</v>
@@ -4246,7 +4240,7 @@
         <v>283</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>9</v>
@@ -4266,10 +4260,10 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>332</v>
+        <v>365</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>27</v>
@@ -4284,13 +4278,13 @@
         <v>247</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>407</v>
+        <v>317</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>408</v>
+        <v>318</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>225</v>
@@ -4302,7 +4296,7 @@
         <v>9</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>365</v>
+        <v>298</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>92</v>
@@ -4310,10 +4304,10 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>333</v>
+        <v>366</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>27</v>
@@ -4328,13 +4322,13 @@
         <v>247</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>407</v>
+        <v>317</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>408</v>
+        <v>318</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>225</v>
@@ -4346,7 +4340,7 @@
         <v>9</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>366</v>
+        <v>299</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>92</v>
@@ -4354,10 +4348,10 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>334</v>
+        <v>367</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>28</v>
@@ -4372,13 +4366,13 @@
         <v>247</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>367</v>
+        <v>300</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>368</v>
+        <v>301</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>87</v>
@@ -4398,10 +4392,10 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>335</v>
+        <v>368</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>28</v>
@@ -4416,13 +4410,13 @@
         <v>247</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>367</v>
+        <v>300</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>368</v>
+        <v>301</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>87</v>
@@ -4442,10 +4436,10 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>300</v>
+        <v>369</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>29</v>
@@ -4466,7 +4460,7 @@
         <v>269</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>95</v>
@@ -4486,10 +4480,10 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>301</v>
+        <v>370</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>29</v>
@@ -4510,7 +4504,7 @@
         <v>269</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>96</v>
@@ -4530,10 +4524,10 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>336</v>
+        <v>371</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>31</v>
@@ -4554,7 +4548,7 @@
         <v>271</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>87</v>
@@ -4574,10 +4568,10 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>337</v>
+        <v>372</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>31</v>
@@ -4598,7 +4592,7 @@
         <v>274</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>87</v>
@@ -4618,10 +4612,10 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>338</v>
+        <v>373</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>31</v>
@@ -4642,7 +4636,7 @@
         <v>274</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>87</v>
@@ -4662,10 +4656,10 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>339</v>
+        <v>374</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>31</v>
@@ -4686,7 +4680,7 @@
         <v>274</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>87</v>
@@ -4706,10 +4700,10 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>31</v>
@@ -4730,7 +4724,7 @@
         <v>274</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>98</v>
@@ -4750,10 +4744,10 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>340</v>
+        <v>376</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>34</v>
@@ -4774,7 +4768,7 @@
         <v>271</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>87</v>
@@ -4794,16 +4788,16 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>341</v>
+        <v>377</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>374</v>
+        <v>303</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>52</v>
@@ -4818,7 +4812,7 @@
         <v>271</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>98</v>
@@ -4838,16 +4832,16 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>302</v>
+        <v>378</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>374</v>
+        <v>303</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>52</v>
@@ -4862,7 +4856,7 @@
         <v>279</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>9</v>
@@ -4882,10 +4876,10 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>342</v>
+        <v>379</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>36</v>
@@ -4906,7 +4900,7 @@
         <v>271</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>98</v>
@@ -4926,10 +4920,10 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>303</v>
+        <v>380</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>36</v>
@@ -4950,7 +4944,7 @@
         <v>279</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>9</v>
@@ -4970,10 +4964,10 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>343</v>
+        <v>381</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>37</v>
@@ -4994,7 +4988,7 @@
         <v>270</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>231</v>
@@ -5014,10 +5008,10 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>344</v>
+        <v>382</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>37</v>
@@ -5038,7 +5032,7 @@
         <v>270</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>231</v>
@@ -5058,10 +5052,10 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>38</v>
@@ -5079,10 +5073,10 @@
         <v>39</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>369</v>
+        <v>302</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>295</v>
@@ -5102,10 +5096,10 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>38</v>
@@ -5123,10 +5117,10 @@
         <v>39</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>369</v>
+        <v>302</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>295</v>
@@ -5146,10 +5140,10 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>38</v>
@@ -5167,10 +5161,10 @@
         <v>39</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>369</v>
+        <v>302</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>295</v>
@@ -5190,10 +5184,10 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>38</v>
@@ -5211,10 +5205,10 @@
         <v>39</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>369</v>
+        <v>302</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>295</v>
@@ -5234,10 +5228,10 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>345</v>
+        <v>387</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>40</v>
@@ -5258,7 +5252,7 @@
         <v>271</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>231</v>
@@ -5278,10 +5272,10 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>346</v>
+        <v>388</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>40</v>
@@ -5302,7 +5296,7 @@
         <v>274</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>231</v>
@@ -5322,10 +5316,10 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>347</v>
+        <v>389</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>40</v>
@@ -5346,7 +5340,7 @@
         <v>274</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>231</v>
@@ -5366,10 +5360,10 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>348</v>
+        <v>390</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>40</v>
@@ -5390,7 +5384,7 @@
         <v>274</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>231</v>
@@ -5410,10 +5404,10 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>40</v>
@@ -5434,7 +5428,7 @@
         <v>274</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>98</v>
@@ -5454,10 +5448,10 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>349</v>
+        <v>392</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>41</v>
@@ -5478,7 +5472,7 @@
         <v>273</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>231</v>
@@ -5498,10 +5492,10 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>42</v>
@@ -5522,7 +5516,7 @@
         <v>273</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>231</v>
@@ -5542,10 +5536,10 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>42</v>
@@ -5566,7 +5560,7 @@
         <v>280</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>9</v>
@@ -5586,10 +5580,10 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>42</v>
@@ -5610,7 +5604,7 @@
         <v>280</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>9</v>
@@ -5630,10 +5624,10 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>42</v>
@@ -5654,7 +5648,7 @@
         <v>280</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>9</v>
@@ -5674,10 +5668,10 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>42</v>
@@ -5698,7 +5692,7 @@
         <v>280</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>9</v>
@@ -5718,10 +5712,10 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>352</v>
+        <v>398</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>44</v>
@@ -5739,10 +5733,10 @@
         <v>45</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>375</v>
+        <v>304</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J81" s="4" t="s">
         <v>231</v>
@@ -5762,10 +5756,10 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>353</v>
+        <v>399</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>44</v>
@@ -5783,10 +5777,10 @@
         <v>45</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>375</v>
+        <v>304</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>231</v>
@@ -5806,10 +5800,10 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>354</v>
+        <v>400</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>46</v>
@@ -5827,10 +5821,10 @@
         <v>47</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>379</v>
+        <v>308</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J83" s="4" t="s">
         <v>295</v>
@@ -5842,7 +5836,7 @@
         <v>9</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>380</v>
+        <v>309</v>
       </c>
       <c r="N83" s="4" t="s">
         <v>92</v>
@@ -5850,10 +5844,10 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>355</v>
+        <v>401</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>46</v>
@@ -5871,10 +5865,10 @@
         <v>47</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>379</v>
+        <v>308</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>295</v>
@@ -5886,7 +5880,7 @@
         <v>9</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>92</v>
@@ -5894,10 +5888,10 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>356</v>
+        <v>402</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>46</v>
@@ -5915,10 +5909,10 @@
         <v>47</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>379</v>
+        <v>308</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J85" s="4" t="s">
         <v>295</v>
@@ -5930,7 +5924,7 @@
         <v>9</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>382</v>
+        <v>311</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>92</v>
@@ -5938,10 +5932,10 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>357</v>
+        <v>403</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>46</v>
@@ -5959,10 +5953,10 @@
         <v>47</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>379</v>
+        <v>308</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J86" s="4" t="s">
         <v>295</v>
@@ -5974,7 +5968,7 @@
         <v>9</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>383</v>
+        <v>312</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>92</v>
@@ -5982,10 +5976,10 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>358</v>
+        <v>404</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>48</v>
@@ -6006,7 +6000,7 @@
         <v>273</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>98</v>
@@ -6018,7 +6012,7 @@
         <v>9</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>376</v>
+        <v>305</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>92</v>
@@ -6026,10 +6020,10 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>359</v>
+        <v>405</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>48</v>
@@ -6050,7 +6044,7 @@
         <v>273</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>98</v>
@@ -6062,7 +6056,7 @@
         <v>9</v>
       </c>
       <c r="M88" s="4" t="s">
-        <v>377</v>
+        <v>306</v>
       </c>
       <c r="N88" s="4" t="s">
         <v>92</v>
@@ -6070,10 +6064,10 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>393</v>
+        <v>406</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>48</v>
@@ -6094,7 +6088,7 @@
         <v>273</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>98</v>
@@ -6106,7 +6100,7 @@
         <v>9</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>377</v>
+        <v>306</v>
       </c>
       <c r="N89" s="4" t="s">
         <v>92</v>
@@ -6114,10 +6108,10 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>360</v>
+        <v>407</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>48</v>
@@ -6138,7 +6132,7 @@
         <v>273</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J90" s="4" t="s">
         <v>98</v>
@@ -6150,7 +6144,7 @@
         <v>9</v>
       </c>
       <c r="M90" s="4" t="s">
-        <v>378</v>
+        <v>307</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>92</v>
@@ -6158,16 +6152,16 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>384</v>
+        <v>408</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>410</v>
+        <v>320</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>385</v>
+        <v>313</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>52</v>
@@ -6182,7 +6176,7 @@
         <v>273</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>409</v>
+        <v>319</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Update other disagg for tb_art
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{311BB2C3-5719-BB40-B037-822E68FB632D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9D0B20AD-A988-0946-8890-775CB9528E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37460" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -2234,10 +2234,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="I89" sqref="A89:I89"/>
+      <selection pane="topRight" activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2736,7 +2736,7 @@
       <c r="L11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N11" s="6" t="s">
@@ -2780,7 +2780,7 @@
       <c r="L12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N12" s="6" t="s">
@@ -2868,7 +2868,7 @@
       <c r="L14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N14" s="6" t="s">
@@ -2912,7 +2912,7 @@
       <c r="L15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N15" s="6" t="s">
@@ -3000,7 +3000,7 @@
       <c r="L17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N17" s="6" t="s">
@@ -3044,7 +3044,7 @@
       <c r="L18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N18" s="6" t="s">
@@ -3088,7 +3088,7 @@
       <c r="L19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N19" s="6" t="s">
@@ -3132,7 +3132,7 @@
       <c r="L20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N20" s="6" t="s">
@@ -3220,7 +3220,7 @@
       <c r="L22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N22" s="6" t="s">
@@ -3264,7 +3264,7 @@
       <c r="L23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N23" s="6" t="s">
@@ -3352,7 +3352,7 @@
       <c r="L25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="M25" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N25" s="6" t="s">
@@ -3396,7 +3396,7 @@
       <c r="L26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M26" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N26" s="6" t="s">
@@ -3484,7 +3484,7 @@
       <c r="L28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="M28" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N28" s="6" t="s">
@@ -3528,7 +3528,7 @@
       <c r="L29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M29" s="4" t="s">
+      <c r="M29" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N29" s="6" t="s">
@@ -3572,7 +3572,7 @@
       <c r="L30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="M30" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N30" s="6" t="s">
@@ -3616,7 +3616,7 @@
       <c r="L31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="M31" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N31" s="6" t="s">
@@ -3704,7 +3704,7 @@
       <c r="L33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M33" s="4" t="s">
+      <c r="M33" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N33" s="6" t="s">
@@ -3748,7 +3748,7 @@
       <c r="L34" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M34" s="4" t="s">
+      <c r="M34" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N34" s="6" t="s">
@@ -3836,7 +3836,7 @@
       <c r="L36" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M36" s="4" t="s">
+      <c r="M36" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N36" s="6" t="s">
@@ -3880,7 +3880,7 @@
       <c r="L37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M37" s="4" t="s">
+      <c r="M37" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N37" s="6" t="s">
@@ -3968,7 +3968,7 @@
       <c r="L39" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M39" s="4" t="s">
+      <c r="M39" s="6" t="s">
         <v>219</v>
       </c>
       <c r="N39" s="6" t="s">
@@ -4012,7 +4012,7 @@
       <c r="L40" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M40" s="4" t="s">
+      <c r="M40" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N40" s="6" t="s">
@@ -4144,7 +4144,7 @@
       <c r="L43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M43" s="4" t="s">
+      <c r="M43" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N43" s="6" t="s">
@@ -4188,7 +4188,7 @@
       <c r="L44" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="M44" s="4" t="s">
+      <c r="M44" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N44" s="6" t="s">
@@ -4364,7 +4364,7 @@
       <c r="L48" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M48" s="4" t="s">
+      <c r="M48" s="6" t="s">
         <v>223</v>
       </c>
       <c r="N48" s="6" t="s">
@@ -4408,7 +4408,7 @@
       <c r="L49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M49" s="4" t="s">
+      <c r="M49" s="6" t="s">
         <v>224</v>
       </c>
       <c r="N49" s="6" t="s">
@@ -4452,7 +4452,7 @@
       <c r="L50" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M50" s="4" t="s">
+      <c r="M50" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N50" s="6" t="s">
@@ -4496,7 +4496,7 @@
       <c r="L51" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M51" s="4" t="s">
+      <c r="M51" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N51" s="6" t="s">
@@ -4540,7 +4540,7 @@
       <c r="L52" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M52" s="4" t="s">
+      <c r="M52" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N52" s="6" t="s">
@@ -4584,7 +4584,7 @@
       <c r="L53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M53" s="4" t="s">
+      <c r="M53" s="6" t="s">
         <v>225</v>
       </c>
       <c r="N53" s="6" t="s">
@@ -4628,7 +4628,7 @@
       <c r="L54" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M54" s="4" t="s">
+      <c r="M54" s="6" t="s">
         <v>226</v>
       </c>
       <c r="N54" s="6" t="s">
@@ -4672,7 +4672,7 @@
       <c r="L55" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M55" s="4" t="s">
+      <c r="M55" s="6" t="s">
         <v>227</v>
       </c>
       <c r="N55" s="6" t="s">
@@ -4760,7 +4760,7 @@
       <c r="L57" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M57" s="4" t="s">
+      <c r="M57" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N57" s="6" t="s">
@@ -4804,7 +4804,7 @@
       <c r="L58" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M58" s="4" t="s">
+      <c r="M58" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N58" s="6" t="s">
@@ -4848,7 +4848,7 @@
       <c r="L59" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M59" s="4" t="s">
+      <c r="M59" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N59" s="6" t="s">
@@ -4892,7 +4892,7 @@
       <c r="L60" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M60" s="4" t="s">
+      <c r="M60" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N60" s="6" t="s">
@@ -4936,7 +4936,7 @@
       <c r="L61" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M61" s="4" t="s">
+      <c r="M61" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N61" s="6" t="s">
@@ -4980,8 +4980,8 @@
       <c r="L62" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M62" s="4" t="s">
-        <v>9</v>
+      <c r="M62" s="6" t="s">
+        <v>223</v>
       </c>
       <c r="N62" s="6" t="s">
         <v>89</v>
@@ -5024,8 +5024,8 @@
       <c r="L63" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M63" s="4" t="s">
-        <v>9</v>
+      <c r="M63" s="6" t="s">
+        <v>224</v>
       </c>
       <c r="N63" s="6" t="s">
         <v>89</v>
@@ -5068,7 +5068,7 @@
       <c r="L64" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M64" s="4" t="s">
+      <c r="M64" s="6" t="s">
         <v>223</v>
       </c>
       <c r="N64" s="6" t="s">
@@ -5112,7 +5112,7 @@
       <c r="L65" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M65" s="4" t="s">
+      <c r="M65" s="6" t="s">
         <v>224</v>
       </c>
       <c r="N65" s="6" t="s">
@@ -5156,7 +5156,7 @@
       <c r="L66" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M66" s="4" t="s">
+      <c r="M66" s="6" t="s">
         <v>223</v>
       </c>
       <c r="N66" s="6" t="s">
@@ -5200,7 +5200,7 @@
       <c r="L67" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M67" s="4" t="s">
+      <c r="M67" s="6" t="s">
         <v>224</v>
       </c>
       <c r="N67" s="6" t="s">
@@ -5244,7 +5244,7 @@
       <c r="L68" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M68" s="4" t="s">
+      <c r="M68" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N68" s="6" t="s">
@@ -5288,7 +5288,7 @@
       <c r="L69" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M69" s="4" t="s">
+      <c r="M69" s="6" t="s">
         <v>225</v>
       </c>
       <c r="N69" s="6" t="s">
@@ -5332,7 +5332,7 @@
       <c r="L70" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M70" s="4" t="s">
+      <c r="M70" s="6" t="s">
         <v>226</v>
       </c>
       <c r="N70" s="6" t="s">
@@ -5376,7 +5376,7 @@
       <c r="L71" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M71" s="4" t="s">
+      <c r="M71" s="6" t="s">
         <v>227</v>
       </c>
       <c r="N71" s="6" t="s">
@@ -5464,7 +5464,7 @@
       <c r="L73" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M73" s="4" t="s">
+      <c r="M73" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N73" s="6" t="s">
@@ -5508,7 +5508,7 @@
       <c r="L74" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M74" s="4" t="s">
+      <c r="M74" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N74" s="6" t="s">
@@ -5552,7 +5552,7 @@
       <c r="L75" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M75" s="4" t="s">
+      <c r="M75" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N75" s="6" t="s">
@@ -5596,7 +5596,7 @@
       <c r="L76" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M76" s="4" t="s">
+      <c r="M76" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N76" s="6" t="s">
@@ -5640,7 +5640,7 @@
       <c r="L77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M77" s="4" t="s">
+      <c r="M77" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N77" s="6" t="s">
@@ -5684,7 +5684,7 @@
       <c r="L78" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M78" s="4" t="s">
+      <c r="M78" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N78" s="6" t="s">
@@ -5728,7 +5728,7 @@
       <c r="L79" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M79" s="4" t="s">
+      <c r="M79" s="6" t="s">
         <v>237</v>
       </c>
       <c r="N79" s="6" t="s">
@@ -5772,7 +5772,7 @@
       <c r="L80" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M80" s="4" t="s">
+      <c r="M80" s="6" t="s">
         <v>237</v>
       </c>
       <c r="N80" s="6" t="s">
@@ -5816,7 +5816,7 @@
       <c r="L81" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M81" s="4" t="s">
+      <c r="M81" s="6" t="s">
         <v>302</v>
       </c>
       <c r="N81" s="6" t="s">
@@ -5860,7 +5860,7 @@
       <c r="L82" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M82" s="4" t="s">
+      <c r="M82" s="6" t="s">
         <v>303</v>
       </c>
       <c r="N82" s="6" t="s">
@@ -5904,7 +5904,7 @@
       <c r="L83" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M83" s="4" t="s">
+      <c r="M83" s="6" t="s">
         <v>304</v>
       </c>
       <c r="N83" s="6" t="s">
@@ -5948,7 +5948,7 @@
       <c r="L84" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M84" s="4" t="s">
+      <c r="M84" s="6" t="s">
         <v>305</v>
       </c>
       <c r="N84" s="6" t="s">
@@ -5992,7 +5992,7 @@
       <c r="L85" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M85" s="4" t="s">
+      <c r="M85" s="6" t="s">
         <v>298</v>
       </c>
       <c r="N85" s="6" t="s">
@@ -6036,7 +6036,7 @@
       <c r="L86" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M86" s="4" t="s">
+      <c r="M86" s="6" t="s">
         <v>299</v>
       </c>
       <c r="N86" s="6" t="s">
@@ -6124,7 +6124,7 @@
       <c r="L88" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M88" s="4" t="s">
+      <c r="M88" s="6" t="s">
         <v>300</v>
       </c>
       <c r="N88" s="6" t="s">
@@ -6168,7 +6168,7 @@
       <c r="L89" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M89" s="5" t="s">
+      <c r="M89" s="10" t="s">
         <v>9</v>
       </c>
       <c r="N89" s="10" t="s">

</xml_diff>

<commit_message>
Update a few PSNUxIM indicator codes
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/21Tto22TMap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{171F45B7-3028-3B40-B5DC-3BDF595503F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6AFF23FD-BF1D-DB47-9DE5-17473A8DC465}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1118,9 +1118,6 @@
     <t>OVC_SERV.Active.T</t>
   </si>
   <si>
-    <t>OVC_SERV.Graduated.T</t>
-  </si>
-  <si>
     <t>PMTCT_ART.Already.T</t>
   </si>
   <si>
@@ -1145,9 +1142,6 @@
     <t>PMTCT_STAT.N.New.Pos.T</t>
   </si>
   <si>
-    <t>HTS_RECENT.PMTCT.T</t>
-  </si>
-  <si>
     <t>PP_PREV.T</t>
   </si>
   <si>
@@ -1332,6 +1326,12 @@
   </si>
   <si>
     <t>5-14</t>
+  </si>
+  <si>
+    <t>HTS_RECENT.PMTCT_STAT.T</t>
+  </si>
+  <si>
+    <t>OVC_SERV.Grad.T</t>
   </si>
 </sst>
 </file>
@@ -1930,7 +1930,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkUp"/>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2242,10 +2251,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="M46" sqref="A46:M48"/>
+      <selection pane="topRight" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2498,7 +2507,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>50</v>
@@ -2507,10 +2516,10 @@
         <v>244</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>312</v>
@@ -2630,7 +2639,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>50</v>
@@ -2639,10 +2648,10 @@
         <v>244</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>312</v>
@@ -2806,7 +2815,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>50</v>
@@ -2815,10 +2824,10 @@
         <v>244</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>312</v>
@@ -2938,7 +2947,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>50</v>
@@ -2947,10 +2956,10 @@
         <v>244</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>312</v>
@@ -3158,7 +3167,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>50</v>
@@ -3167,10 +3176,10 @@
         <v>244</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>312</v>
@@ -3290,7 +3299,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>50</v>
@@ -3299,10 +3308,10 @@
         <v>244</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>312</v>
@@ -3422,7 +3431,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>50</v>
@@ -3431,10 +3440,10 @@
         <v>244</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>312</v>
@@ -3642,7 +3651,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>50</v>
@@ -3651,10 +3660,10 @@
         <v>244</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>312</v>
@@ -3774,7 +3783,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>50</v>
@@ -3783,10 +3792,10 @@
         <v>244</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>312</v>
@@ -3906,7 +3915,7 @@
         <v>13</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>50</v>
@@ -3915,10 +3924,10 @@
         <v>244</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>312</v>
@@ -4082,7 +4091,7 @@
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>50</v>
@@ -4116,7 +4125,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="10" t="s">
         <v>355</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -4160,7 +4169,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="10" t="s">
         <v>356</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -4204,7 +4213,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="10" t="s">
         <v>357</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -4293,7 +4302,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>359</v>
+        <v>430</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>313</v>
@@ -4337,7 +4346,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>313</v>
@@ -4364,7 +4373,7 @@
         <v>312</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K48" s="10" t="s">
         <v>85</v>
@@ -4380,8 +4389,8 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>360</v>
+      <c r="A49" s="10" t="s">
+        <v>359</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>313</v>
@@ -4425,7 +4434,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>313</v>
@@ -4469,7 +4478,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>313</v>
@@ -4513,7 +4522,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>313</v>
@@ -4557,7 +4566,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>313</v>
@@ -4601,7 +4610,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>313</v>
@@ -4645,7 +4654,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>313</v>
@@ -4689,7 +4698,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>313</v>
@@ -4732,8 +4741,8 @@
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
-        <v>368</v>
+      <c r="A57" s="6" t="s">
+        <v>429</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>313</v>
@@ -4742,19 +4751,19 @@
         <v>13</v>
       </c>
       <c r="D57" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="H57" s="8" t="s">
         <v>402</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>404</v>
       </c>
       <c r="I57" s="6" t="s">
         <v>312</v>
@@ -4777,7 +4786,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>313</v>
@@ -4821,7 +4830,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>313</v>
@@ -4865,7 +4874,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>313</v>
@@ -4909,7 +4918,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>313</v>
@@ -4953,7 +4962,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>313</v>
@@ -4997,7 +5006,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>313</v>
@@ -5041,7 +5050,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>313</v>
@@ -5085,7 +5094,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>313</v>
@@ -5129,7 +5138,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>313</v>
@@ -5173,7 +5182,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>313</v>
@@ -5217,7 +5226,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>313</v>
@@ -5261,7 +5270,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>313</v>
@@ -5305,7 +5314,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>313</v>
@@ -5349,7 +5358,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>313</v>
@@ -5393,7 +5402,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>313</v>
@@ -5437,7 +5446,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>313</v>
@@ -5446,7 +5455,7 @@
         <v>13</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>50</v>
@@ -5455,10 +5464,10 @@
         <v>244</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I73" s="6" t="s">
         <v>312</v>
@@ -5481,7 +5490,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>313</v>
@@ -5525,7 +5534,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>313</v>
@@ -5569,7 +5578,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>313</v>
@@ -5613,7 +5622,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>313</v>
@@ -5657,7 +5666,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>313</v>
@@ -5701,7 +5710,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>313</v>
@@ -5745,7 +5754,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>313</v>
@@ -5789,7 +5798,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>313</v>
@@ -5833,7 +5842,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>313</v>
@@ -5877,7 +5886,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>313</v>
@@ -5921,7 +5930,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>313</v>
@@ -5965,7 +5974,7 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>313</v>
@@ -6009,7 +6018,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>313</v>
@@ -6053,7 +6062,7 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>313</v>
@@ -6097,7 +6106,7 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>313</v>
@@ -6106,7 +6115,7 @@
         <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>50</v>
@@ -6115,10 +6124,10 @@
         <v>244</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I88" s="6" t="s">
         <v>312</v>
@@ -6141,7 +6150,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>313</v>
@@ -6185,7 +6194,7 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>313</v>
@@ -6233,6 +6242,11 @@
     <sortCondition ref="A2:A90"/>
   </sortState>
   <phoneticPr fontId="19" type="noConversion"/>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$D57="Male"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>